<commit_message>
added polynomial svm results
</commit_message>
<xml_diff>
--- a/testing/Confusion Matrices results.xlsx
+++ b/testing/Confusion Matrices results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12780" windowHeight="7140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12780" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Kernel Perceptron Polynomial: d=5 normalized</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>SVM Kernel  - gamma (ɣ) = 2 / σ = 0.5</t>
+  </si>
+  <si>
+    <t>SVM Polynomial Kernel  (d = 5)</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -171,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,6 +245,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE59" sqref="AE59"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N68" sqref="N68:X79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4492,6 +4504,19 @@
       <c r="I68" s="25"/>
       <c r="J68" s="25"/>
       <c r="K68" s="25"/>
+      <c r="N68" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="O68" s="25"/>
+      <c r="P68" s="25"/>
+      <c r="Q68" s="25"/>
+      <c r="R68" s="25"/>
+      <c r="S68" s="25"/>
+      <c r="T68" s="25"/>
+      <c r="U68" s="25"/>
+      <c r="V68" s="25"/>
+      <c r="W68" s="25"/>
+      <c r="X68" s="25"/>
     </row>
     <row r="69" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
@@ -4525,6 +4550,37 @@
       <c r="K69" s="18">
         <v>9</v>
       </c>
+      <c r="N69" s="19"/>
+      <c r="O69" s="18">
+        <v>0</v>
+      </c>
+      <c r="P69" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="18">
+        <v>2</v>
+      </c>
+      <c r="R69" s="18">
+        <v>3</v>
+      </c>
+      <c r="S69" s="18">
+        <v>4</v>
+      </c>
+      <c r="T69" s="18">
+        <v>5</v>
+      </c>
+      <c r="U69" s="18">
+        <v>6</v>
+      </c>
+      <c r="V69" s="18">
+        <v>7</v>
+      </c>
+      <c r="W69" s="18">
+        <v>8</v>
+      </c>
+      <c r="X69" s="18">
+        <v>9</v>
+      </c>
     </row>
     <row r="70" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="18">
@@ -4560,6 +4616,39 @@
       <c r="K70" s="2">
         <v>0</v>
       </c>
+      <c r="N70" s="18">
+        <v>0</v>
+      </c>
+      <c r="O70" s="26">
+        <v>178</v>
+      </c>
+      <c r="P70" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="2">
+        <v>0</v>
+      </c>
+      <c r="R70" s="2">
+        <v>0</v>
+      </c>
+      <c r="S70" s="2">
+        <v>0</v>
+      </c>
+      <c r="T70" s="2">
+        <v>0</v>
+      </c>
+      <c r="U70" s="2">
+        <v>0</v>
+      </c>
+      <c r="V70" s="2">
+        <v>0</v>
+      </c>
+      <c r="W70" s="2">
+        <v>0</v>
+      </c>
+      <c r="X70" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18">
@@ -4595,6 +4684,39 @@
       <c r="K71" s="2">
         <v>1</v>
       </c>
+      <c r="N71" s="18">
+        <v>1</v>
+      </c>
+      <c r="O71" s="2">
+        <v>0</v>
+      </c>
+      <c r="P71" s="26">
+        <v>182</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>1</v>
+      </c>
+      <c r="R71" s="2">
+        <v>0</v>
+      </c>
+      <c r="S71" s="2">
+        <v>1</v>
+      </c>
+      <c r="T71" s="2">
+        <v>0</v>
+      </c>
+      <c r="U71" s="2">
+        <v>0</v>
+      </c>
+      <c r="V71" s="2">
+        <v>0</v>
+      </c>
+      <c r="W71" s="2">
+        <v>5</v>
+      </c>
+      <c r="X71" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18">
@@ -4628,6 +4750,39 @@
         <v>0</v>
       </c>
       <c r="K72" s="2">
+        <v>0</v>
+      </c>
+      <c r="N72" s="18">
+        <v>2</v>
+      </c>
+      <c r="O72" s="2">
+        <v>0</v>
+      </c>
+      <c r="P72" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="26">
+        <v>176</v>
+      </c>
+      <c r="R72" s="2">
+        <v>0</v>
+      </c>
+      <c r="S72" s="2">
+        <v>0</v>
+      </c>
+      <c r="T72" s="2">
+        <v>0</v>
+      </c>
+      <c r="U72" s="2">
+        <v>0</v>
+      </c>
+      <c r="V72" s="2">
+        <v>0</v>
+      </c>
+      <c r="W72" s="2">
+        <v>0</v>
+      </c>
+      <c r="X72" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4665,6 +4820,39 @@
       <c r="K73" s="2">
         <v>2</v>
       </c>
+      <c r="N73" s="18">
+        <v>3</v>
+      </c>
+      <c r="O73" s="2">
+        <v>0</v>
+      </c>
+      <c r="P73" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="2">
+        <v>0</v>
+      </c>
+      <c r="R73" s="26">
+        <v>178</v>
+      </c>
+      <c r="S73" s="2">
+        <v>0</v>
+      </c>
+      <c r="T73" s="2">
+        <v>0</v>
+      </c>
+      <c r="U73" s="2">
+        <v>0</v>
+      </c>
+      <c r="V73" s="2">
+        <v>0</v>
+      </c>
+      <c r="W73" s="2">
+        <v>0</v>
+      </c>
+      <c r="X73" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18">
@@ -4700,6 +4888,39 @@
       <c r="K74" s="2">
         <v>0</v>
       </c>
+      <c r="N74" s="18">
+        <v>4</v>
+      </c>
+      <c r="O74" s="2">
+        <v>0</v>
+      </c>
+      <c r="P74" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="2">
+        <v>0</v>
+      </c>
+      <c r="R74" s="2">
+        <v>0</v>
+      </c>
+      <c r="S74" s="26">
+        <v>180</v>
+      </c>
+      <c r="T74" s="2">
+        <v>0</v>
+      </c>
+      <c r="U74" s="2">
+        <v>0</v>
+      </c>
+      <c r="V74" s="2">
+        <v>0</v>
+      </c>
+      <c r="W74" s="2">
+        <v>0</v>
+      </c>
+      <c r="X74" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="18">
@@ -4735,6 +4956,39 @@
       <c r="K75" s="2">
         <v>1</v>
       </c>
+      <c r="N75" s="18">
+        <v>5</v>
+      </c>
+      <c r="O75" s="2">
+        <v>0</v>
+      </c>
+      <c r="P75" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>0</v>
+      </c>
+      <c r="R75" s="2">
+        <v>1</v>
+      </c>
+      <c r="S75" s="2">
+        <v>0</v>
+      </c>
+      <c r="T75" s="26">
+        <v>181</v>
+      </c>
+      <c r="U75" s="2">
+        <v>0</v>
+      </c>
+      <c r="V75" s="2">
+        <v>1</v>
+      </c>
+      <c r="W75" s="2">
+        <v>1</v>
+      </c>
+      <c r="X75" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18">
@@ -4770,6 +5024,39 @@
       <c r="K76" s="2">
         <v>0</v>
       </c>
+      <c r="N76" s="18">
+        <v>6</v>
+      </c>
+      <c r="O76" s="2">
+        <v>0</v>
+      </c>
+      <c r="P76" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="2">
+        <v>0</v>
+      </c>
+      <c r="R76" s="2">
+        <v>0</v>
+      </c>
+      <c r="S76" s="2">
+        <v>0</v>
+      </c>
+      <c r="T76" s="2">
+        <v>0</v>
+      </c>
+      <c r="U76" s="26">
+        <v>180</v>
+      </c>
+      <c r="V76" s="2">
+        <v>0</v>
+      </c>
+      <c r="W76" s="2">
+        <v>0</v>
+      </c>
+      <c r="X76" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18">
@@ -4805,6 +5092,39 @@
       <c r="K77" s="2">
         <v>0</v>
       </c>
+      <c r="N77" s="18">
+        <v>7</v>
+      </c>
+      <c r="O77" s="2">
+        <v>0</v>
+      </c>
+      <c r="P77" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="2">
+        <v>0</v>
+      </c>
+      <c r="R77" s="2">
+        <v>1</v>
+      </c>
+      <c r="S77" s="2">
+        <v>0</v>
+      </c>
+      <c r="T77" s="2">
+        <v>0</v>
+      </c>
+      <c r="U77" s="2">
+        <v>0</v>
+      </c>
+      <c r="V77" s="26">
+        <v>174</v>
+      </c>
+      <c r="W77" s="2">
+        <v>0</v>
+      </c>
+      <c r="X77" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
@@ -4840,6 +5160,39 @@
       <c r="K78" s="2">
         <v>2</v>
       </c>
+      <c r="N78" s="18">
+        <v>8</v>
+      </c>
+      <c r="O78" s="2">
+        <v>0</v>
+      </c>
+      <c r="P78" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="2">
+        <v>0</v>
+      </c>
+      <c r="R78" s="2">
+        <v>1</v>
+      </c>
+      <c r="S78" s="2">
+        <v>0</v>
+      </c>
+      <c r="T78" s="2">
+        <v>0</v>
+      </c>
+      <c r="U78" s="2">
+        <v>1</v>
+      </c>
+      <c r="V78" s="2">
+        <v>0</v>
+      </c>
+      <c r="W78" s="26">
+        <v>166</v>
+      </c>
+      <c r="X78" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="79" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18">
@@ -4875,20 +5228,54 @@
       <c r="K79" s="3">
         <v>174</v>
       </c>
+      <c r="N79" s="18">
+        <v>9</v>
+      </c>
+      <c r="O79" s="2">
+        <v>0</v>
+      </c>
+      <c r="P79" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="2">
+        <v>0</v>
+      </c>
+      <c r="R79" s="2">
+        <v>2</v>
+      </c>
+      <c r="S79" s="2">
+        <v>0</v>
+      </c>
+      <c r="T79" s="2">
+        <v>1</v>
+      </c>
+      <c r="U79" s="2">
+        <v>0</v>
+      </c>
+      <c r="V79" s="2">
+        <v>4</v>
+      </c>
+      <c r="W79" s="2">
+        <v>2</v>
+      </c>
+      <c r="X79" s="26">
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="N54:X54"/>
-    <mergeCell ref="N28:X28"/>
-    <mergeCell ref="N41:X41"/>
+  <mergeCells count="12">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="N1:X1"/>
     <mergeCell ref="A41:K41"/>
     <mergeCell ref="N15:X15"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="N54:X54"/>
+    <mergeCell ref="N28:X28"/>
+    <mergeCell ref="N41:X41"/>
+    <mergeCell ref="N68:X68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4897,10 +5284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y83"/>
+  <dimension ref="A1:Y84"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="K83" sqref="B74:K83"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="Z85" sqref="Z85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8864,7 +9251,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="16">
-        <f>SUM(B60:K60)</f>
+        <f t="shared" ref="L60:L70" si="16">SUM(B60:K60)</f>
         <v>175</v>
       </c>
       <c r="N60" s="18">
@@ -8901,7 +9288,7 @@
         <v>0</v>
       </c>
       <c r="Y60" s="16">
-        <f>SUM(O60:X60)</f>
+        <f t="shared" ref="Y60:Y70" si="17">SUM(O60:X60)</f>
         <v>177</v>
       </c>
     </row>
@@ -8940,7 +9327,7 @@
         <v>3</v>
       </c>
       <c r="L61" s="16">
-        <f>SUM(B61:K61)</f>
+        <f t="shared" si="16"/>
         <v>181</v>
       </c>
       <c r="N61" s="18">
@@ -8977,7 +9364,7 @@
         <v>1</v>
       </c>
       <c r="Y61" s="16">
-        <f>SUM(O61:X61)</f>
+        <f t="shared" si="17"/>
         <v>189</v>
       </c>
     </row>
@@ -9016,7 +9403,7 @@
         <v>1</v>
       </c>
       <c r="L62" s="16">
-        <f>SUM(B62:K62)</f>
+        <f t="shared" si="16"/>
         <v>195</v>
       </c>
       <c r="N62" s="18">
@@ -9053,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="Y62" s="16">
-        <f>SUM(O62:X62)</f>
+        <f t="shared" si="17"/>
         <v>172</v>
       </c>
     </row>
@@ -9092,7 +9479,7 @@
         <v>4</v>
       </c>
       <c r="L63" s="16">
-        <f>SUM(B63:K63)</f>
+        <f t="shared" si="16"/>
         <v>173</v>
       </c>
       <c r="N63" s="18">
@@ -9129,7 +9516,7 @@
         <v>2</v>
       </c>
       <c r="Y63" s="16">
-        <f>SUM(O63:X63)</f>
+        <f t="shared" si="17"/>
         <v>179</v>
       </c>
     </row>
@@ -9168,7 +9555,7 @@
         <v>5</v>
       </c>
       <c r="L64" s="16">
-        <f>SUM(B64:K64)</f>
+        <f t="shared" si="16"/>
         <v>180</v>
       </c>
       <c r="N64" s="18">
@@ -9205,7 +9592,7 @@
         <v>0</v>
       </c>
       <c r="Y64" s="16">
-        <f>SUM(O64:X64)</f>
+        <f t="shared" si="17"/>
         <v>181</v>
       </c>
     </row>
@@ -9244,7 +9631,7 @@
         <v>3</v>
       </c>
       <c r="L65" s="16">
-        <f>SUM(B65:K65)</f>
+        <f t="shared" si="16"/>
         <v>202</v>
       </c>
       <c r="N65" s="18">
@@ -9281,7 +9668,7 @@
         <v>1</v>
       </c>
       <c r="Y65" s="16">
-        <f>SUM(O65:X65)</f>
+        <f t="shared" si="17"/>
         <v>182</v>
       </c>
     </row>
@@ -9320,7 +9707,7 @@
         <v>0</v>
       </c>
       <c r="L66" s="16">
-        <f>SUM(B66:K66)</f>
+        <f t="shared" si="16"/>
         <v>181</v>
       </c>
       <c r="N66" s="18">
@@ -9357,7 +9744,7 @@
         <v>0</v>
       </c>
       <c r="Y66" s="16">
-        <f>SUM(O66:X66)</f>
+        <f t="shared" si="17"/>
         <v>180</v>
       </c>
     </row>
@@ -9396,7 +9783,7 @@
         <v>0</v>
       </c>
       <c r="L67" s="16">
-        <f>SUM(B67:K67)</f>
+        <f t="shared" si="16"/>
         <v>172</v>
       </c>
       <c r="N67" s="18">
@@ -9433,7 +9820,7 @@
         <v>0</v>
       </c>
       <c r="Y67" s="16">
-        <f>SUM(O67:X67)</f>
+        <f t="shared" si="17"/>
         <v>178</v>
       </c>
     </row>
@@ -9472,7 +9859,7 @@
         <v>4</v>
       </c>
       <c r="L68" s="16">
-        <f>SUM(B68:K68)</f>
+        <f t="shared" si="16"/>
         <v>156</v>
       </c>
       <c r="N68" s="18">
@@ -9509,7 +9896,7 @@
         <v>2</v>
       </c>
       <c r="Y68" s="16">
-        <f>SUM(O68:X68)</f>
+        <f t="shared" si="17"/>
         <v>178</v>
       </c>
     </row>
@@ -9548,7 +9935,7 @@
         <v>160</v>
       </c>
       <c r="L69" s="16">
-        <f>SUM(B69:K69)</f>
+        <f t="shared" si="16"/>
         <v>182</v>
       </c>
       <c r="N69" s="18">
@@ -9585,97 +9972,97 @@
         <v>174</v>
       </c>
       <c r="Y69" s="16">
-        <f>SUM(O69:X69)</f>
+        <f t="shared" si="17"/>
         <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1">
-        <f>SUM(B60:B69)</f>
+        <f t="shared" ref="B70:K70" si="18">SUM(B60:B69)</f>
         <v>178</v>
       </c>
       <c r="C70" s="1">
-        <f>SUM(C60:C69)</f>
+        <f t="shared" si="18"/>
         <v>182</v>
       </c>
       <c r="D70" s="1">
-        <f>SUM(D60:D69)</f>
+        <f t="shared" si="18"/>
         <v>177</v>
       </c>
       <c r="E70" s="1">
-        <f>SUM(E60:E69)</f>
+        <f t="shared" si="18"/>
         <v>183</v>
       </c>
       <c r="F70" s="1">
-        <f>SUM(F60:F69)</f>
+        <f t="shared" si="18"/>
         <v>181</v>
       </c>
       <c r="G70" s="1">
-        <f>SUM(G60:G69)</f>
+        <f t="shared" si="18"/>
         <v>182</v>
       </c>
       <c r="H70" s="1">
-        <f>SUM(H60:H69)</f>
+        <f t="shared" si="18"/>
         <v>181</v>
       </c>
       <c r="I70" s="1">
-        <f>SUM(I60:I69)</f>
+        <f t="shared" si="18"/>
         <v>179</v>
       </c>
       <c r="J70" s="1">
-        <f>SUM(J60:J69)</f>
+        <f t="shared" si="18"/>
         <v>174</v>
       </c>
       <c r="K70" s="1">
-        <f>SUM(K60:K69)</f>
+        <f t="shared" si="18"/>
         <v>180</v>
       </c>
       <c r="L70" s="16">
-        <f>SUM(B70:K70)</f>
+        <f t="shared" si="16"/>
         <v>1797</v>
       </c>
       <c r="O70" s="1">
-        <f>SUM(O60:O69)</f>
+        <f t="shared" ref="O70:X70" si="19">SUM(O60:O69)</f>
         <v>178</v>
       </c>
       <c r="P70" s="1">
-        <f>SUM(P60:P69)</f>
+        <f t="shared" si="19"/>
         <v>182</v>
       </c>
       <c r="Q70" s="1">
-        <f>SUM(Q60:Q69)</f>
+        <f t="shared" si="19"/>
         <v>177</v>
       </c>
       <c r="R70" s="1">
-        <f>SUM(R60:R69)</f>
+        <f t="shared" si="19"/>
         <v>183</v>
       </c>
       <c r="S70" s="1">
-        <f>SUM(S60:S69)</f>
+        <f t="shared" si="19"/>
         <v>181</v>
       </c>
       <c r="T70" s="1">
-        <f>SUM(T60:T69)</f>
+        <f t="shared" si="19"/>
         <v>182</v>
       </c>
       <c r="U70" s="1">
-        <f>SUM(U60:U69)</f>
+        <f t="shared" si="19"/>
         <v>181</v>
       </c>
       <c r="V70" s="1">
-        <f>SUM(V60:V69)</f>
+        <f t="shared" si="19"/>
         <v>179</v>
       </c>
       <c r="W70" s="1">
-        <f>SUM(W60:W69)</f>
+        <f t="shared" si="19"/>
         <v>174</v>
       </c>
       <c r="X70" s="1">
-        <f>SUM(X60:X69)</f>
+        <f t="shared" si="19"/>
         <v>180</v>
       </c>
       <c r="Y70" s="16">
-        <f>SUM(O70:X70)</f>
+        <f t="shared" si="17"/>
         <v>1797</v>
       </c>
     </row>
@@ -9693,6 +10080,19 @@
       <c r="I72" s="25"/>
       <c r="J72" s="25"/>
       <c r="K72" s="25"/>
+      <c r="N72" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="O72" s="25"/>
+      <c r="P72" s="25"/>
+      <c r="Q72" s="25"/>
+      <c r="R72" s="25"/>
+      <c r="S72" s="25"/>
+      <c r="T72" s="25"/>
+      <c r="U72" s="25"/>
+      <c r="V72" s="25"/>
+      <c r="W72" s="25"/>
+      <c r="X72" s="25"/>
     </row>
     <row r="73" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
@@ -9726,6 +10126,37 @@
       <c r="K73" s="18">
         <v>9</v>
       </c>
+      <c r="N73" s="19"/>
+      <c r="O73" s="18">
+        <v>0</v>
+      </c>
+      <c r="P73" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="18">
+        <v>2</v>
+      </c>
+      <c r="R73" s="18">
+        <v>3</v>
+      </c>
+      <c r="S73" s="18">
+        <v>4</v>
+      </c>
+      <c r="T73" s="18">
+        <v>5</v>
+      </c>
+      <c r="U73" s="18">
+        <v>6</v>
+      </c>
+      <c r="V73" s="18">
+        <v>7</v>
+      </c>
+      <c r="W73" s="18">
+        <v>8</v>
+      </c>
+      <c r="X73" s="18">
+        <v>9</v>
+      </c>
     </row>
     <row r="74" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18">
@@ -9761,6 +10192,43 @@
       <c r="K74" s="7">
         <v>0</v>
       </c>
+      <c r="N74" s="18">
+        <v>0</v>
+      </c>
+      <c r="O74" s="26">
+        <v>178</v>
+      </c>
+      <c r="P74" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="2">
+        <v>0</v>
+      </c>
+      <c r="R74" s="2">
+        <v>0</v>
+      </c>
+      <c r="S74" s="2">
+        <v>0</v>
+      </c>
+      <c r="T74" s="2">
+        <v>0</v>
+      </c>
+      <c r="U74" s="2">
+        <v>0</v>
+      </c>
+      <c r="V74" s="2">
+        <v>0</v>
+      </c>
+      <c r="W74" s="2">
+        <v>0</v>
+      </c>
+      <c r="X74" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y74" s="1">
+        <f>SUM(O74:X74)</f>
+        <v>178</v>
+      </c>
     </row>
     <row r="75" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="18">
@@ -9796,6 +10264,43 @@
       <c r="K75" s="7">
         <v>0</v>
       </c>
+      <c r="N75" s="18">
+        <v>1</v>
+      </c>
+      <c r="O75" s="2">
+        <v>0</v>
+      </c>
+      <c r="P75" s="26">
+        <v>182</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>1</v>
+      </c>
+      <c r="R75" s="2">
+        <v>0</v>
+      </c>
+      <c r="S75" s="2">
+        <v>1</v>
+      </c>
+      <c r="T75" s="2">
+        <v>0</v>
+      </c>
+      <c r="U75" s="2">
+        <v>0</v>
+      </c>
+      <c r="V75" s="2">
+        <v>0</v>
+      </c>
+      <c r="W75" s="2">
+        <v>5</v>
+      </c>
+      <c r="X75" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y75" s="1">
+        <f>SUM(O75:X75)</f>
+        <v>190</v>
+      </c>
     </row>
     <row r="76" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18">
@@ -9830,6 +10335,43 @@
       </c>
       <c r="K76" s="7">
         <v>0</v>
+      </c>
+      <c r="N76" s="18">
+        <v>2</v>
+      </c>
+      <c r="O76" s="2">
+        <v>0</v>
+      </c>
+      <c r="P76" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="26">
+        <v>176</v>
+      </c>
+      <c r="R76" s="2">
+        <v>0</v>
+      </c>
+      <c r="S76" s="2">
+        <v>0</v>
+      </c>
+      <c r="T76" s="2">
+        <v>0</v>
+      </c>
+      <c r="U76" s="2">
+        <v>0</v>
+      </c>
+      <c r="V76" s="2">
+        <v>0</v>
+      </c>
+      <c r="W76" s="2">
+        <v>0</v>
+      </c>
+      <c r="X76" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y76" s="1">
+        <f>SUM(O76:X76)</f>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9866,6 +10408,43 @@
       <c r="K77" s="7">
         <v>180</v>
       </c>
+      <c r="N77" s="18">
+        <v>3</v>
+      </c>
+      <c r="O77" s="2">
+        <v>0</v>
+      </c>
+      <c r="P77" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="2">
+        <v>0</v>
+      </c>
+      <c r="R77" s="26">
+        <v>178</v>
+      </c>
+      <c r="S77" s="2">
+        <v>0</v>
+      </c>
+      <c r="T77" s="2">
+        <v>0</v>
+      </c>
+      <c r="U77" s="2">
+        <v>0</v>
+      </c>
+      <c r="V77" s="2">
+        <v>0</v>
+      </c>
+      <c r="W77" s="2">
+        <v>0</v>
+      </c>
+      <c r="X77" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y77" s="1">
+        <f>SUM(O77:X77)</f>
+        <v>179</v>
+      </c>
     </row>
     <row r="78" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
@@ -9901,6 +10480,43 @@
       <c r="K78" s="7">
         <v>0</v>
       </c>
+      <c r="N78" s="18">
+        <v>4</v>
+      </c>
+      <c r="O78" s="2">
+        <v>0</v>
+      </c>
+      <c r="P78" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="2">
+        <v>0</v>
+      </c>
+      <c r="R78" s="2">
+        <v>0</v>
+      </c>
+      <c r="S78" s="26">
+        <v>180</v>
+      </c>
+      <c r="T78" s="2">
+        <v>0</v>
+      </c>
+      <c r="U78" s="2">
+        <v>0</v>
+      </c>
+      <c r="V78" s="2">
+        <v>0</v>
+      </c>
+      <c r="W78" s="2">
+        <v>0</v>
+      </c>
+      <c r="X78" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="1">
+        <f>SUM(O78:X78)</f>
+        <v>180</v>
+      </c>
     </row>
     <row r="79" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18">
@@ -9936,6 +10552,43 @@
       <c r="K79" s="7">
         <v>0</v>
       </c>
+      <c r="N79" s="18">
+        <v>5</v>
+      </c>
+      <c r="O79" s="2">
+        <v>0</v>
+      </c>
+      <c r="P79" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="2">
+        <v>0</v>
+      </c>
+      <c r="R79" s="2">
+        <v>1</v>
+      </c>
+      <c r="S79" s="2">
+        <v>0</v>
+      </c>
+      <c r="T79" s="26">
+        <v>181</v>
+      </c>
+      <c r="U79" s="2">
+        <v>0</v>
+      </c>
+      <c r="V79" s="2">
+        <v>1</v>
+      </c>
+      <c r="W79" s="2">
+        <v>1</v>
+      </c>
+      <c r="X79" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y79" s="1">
+        <f>SUM(O79:X79)</f>
+        <v>185</v>
+      </c>
     </row>
     <row r="80" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
@@ -9971,8 +10624,45 @@
       <c r="K80" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N80" s="18">
+        <v>6</v>
+      </c>
+      <c r="O80" s="2">
+        <v>0</v>
+      </c>
+      <c r="P80" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="2">
+        <v>0</v>
+      </c>
+      <c r="R80" s="2">
+        <v>0</v>
+      </c>
+      <c r="S80" s="2">
+        <v>0</v>
+      </c>
+      <c r="T80" s="2">
+        <v>0</v>
+      </c>
+      <c r="U80" s="26">
+        <v>180</v>
+      </c>
+      <c r="V80" s="2">
+        <v>0</v>
+      </c>
+      <c r="W80" s="2">
+        <v>0</v>
+      </c>
+      <c r="X80" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y80" s="1">
+        <f>SUM(O80:X80)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18">
         <v>7</v>
       </c>
@@ -10006,8 +10696,45 @@
       <c r="K81" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N81" s="18">
+        <v>7</v>
+      </c>
+      <c r="O81" s="2">
+        <v>0</v>
+      </c>
+      <c r="P81" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="2">
+        <v>0</v>
+      </c>
+      <c r="R81" s="2">
+        <v>1</v>
+      </c>
+      <c r="S81" s="2">
+        <v>0</v>
+      </c>
+      <c r="T81" s="2">
+        <v>0</v>
+      </c>
+      <c r="U81" s="2">
+        <v>0</v>
+      </c>
+      <c r="V81" s="26">
+        <v>174</v>
+      </c>
+      <c r="W81" s="2">
+        <v>0</v>
+      </c>
+      <c r="X81" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y81" s="1">
+        <f>SUM(O81:X81)</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
         <v>8</v>
       </c>
@@ -10041,8 +10768,45 @@
       <c r="K82" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N82" s="18">
+        <v>8</v>
+      </c>
+      <c r="O82" s="2">
+        <v>0</v>
+      </c>
+      <c r="P82" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="2">
+        <v>0</v>
+      </c>
+      <c r="R82" s="2">
+        <v>1</v>
+      </c>
+      <c r="S82" s="2">
+        <v>0</v>
+      </c>
+      <c r="T82" s="2">
+        <v>0</v>
+      </c>
+      <c r="U82" s="2">
+        <v>1</v>
+      </c>
+      <c r="V82" s="2">
+        <v>0</v>
+      </c>
+      <c r="W82" s="26">
+        <v>166</v>
+      </c>
+      <c r="X82" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y82" s="1">
+        <f>SUM(O82:X82)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="18">
         <v>9</v>
       </c>
@@ -10076,20 +10840,104 @@
       <c r="K83" s="7">
         <v>0</v>
       </c>
+      <c r="N83" s="18">
+        <v>9</v>
+      </c>
+      <c r="O83" s="2">
+        <v>0</v>
+      </c>
+      <c r="P83" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="2">
+        <v>0</v>
+      </c>
+      <c r="R83" s="2">
+        <v>2</v>
+      </c>
+      <c r="S83" s="2">
+        <v>0</v>
+      </c>
+      <c r="T83" s="2">
+        <v>1</v>
+      </c>
+      <c r="U83" s="2">
+        <v>0</v>
+      </c>
+      <c r="V83" s="2">
+        <v>4</v>
+      </c>
+      <c r="W83" s="2">
+        <v>2</v>
+      </c>
+      <c r="X83" s="26">
+        <v>175</v>
+      </c>
+      <c r="Y83" s="1">
+        <f>SUM(O83:X83)</f>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O84" s="1">
+        <f>SUM(O74:O83)</f>
+        <v>178</v>
+      </c>
+      <c r="P84" s="1">
+        <f>SUM(P74:P83)</f>
+        <v>182</v>
+      </c>
+      <c r="Q84" s="1">
+        <f>SUM(Q74:Q83)</f>
+        <v>177</v>
+      </c>
+      <c r="R84" s="1">
+        <f>SUM(R74:R83)</f>
+        <v>183</v>
+      </c>
+      <c r="S84" s="1">
+        <f>SUM(S74:S83)</f>
+        <v>181</v>
+      </c>
+      <c r="T84" s="1">
+        <f>SUM(T74:T83)</f>
+        <v>182</v>
+      </c>
+      <c r="U84" s="1">
+        <f>SUM(U74:U83)</f>
+        <v>181</v>
+      </c>
+      <c r="V84" s="1">
+        <f>SUM(V74:V83)</f>
+        <v>179</v>
+      </c>
+      <c r="W84" s="1">
+        <f>SUM(W74:W83)</f>
+        <v>174</v>
+      </c>
+      <c r="X84" s="1">
+        <f>SUM(X74:X83)</f>
+        <v>180</v>
+      </c>
+      <c r="Y84" s="1">
+        <f>SUM(O84:X84)</f>
+        <v>1797</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="N58:X58"/>
-    <mergeCell ref="A72:K72"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="N43:X43"/>
+  <mergeCells count="12">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="N1:X1"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="N15:X15"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="N29:X29"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="N58:X58"/>
+    <mergeCell ref="A72:K72"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="N43:X43"/>
+    <mergeCell ref="N72:X72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
unsaved changes from last commit
</commit_message>
<xml_diff>
--- a/testing/Confusion Matrices results.xlsx
+++ b/testing/Confusion Matrices results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cn262114\Documents\eclipse-workspace\ML_A2\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chinmaya\Documents\eclipse-workspace\ML_A2_github\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Kernel Perceptron Polynomial: d=5 normalized</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>SVM Polynomial Kernel  (d = 5)</t>
+  </si>
+  <si>
+    <t>SuccessCount: 659 TotalCount: 1000</t>
+  </si>
+  <si>
+    <t>Total accuracies: 65.9</t>
   </si>
 </sst>
 </file>
@@ -180,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -244,10 +250,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,43 +545,43 @@
       <selection activeCell="N68" sqref="N68:X79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="11" width="4.140625" style="1"/>
-    <col min="12" max="12" width="4.140625" style="16"/>
-    <col min="13" max="16384" width="4.140625" style="1"/>
+    <col min="1" max="11" width="4.1796875" style="1"/>
+    <col min="12" max="12" width="4.1796875" style="16"/>
+    <col min="13" max="16384" width="4.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+    <row r="1" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="13"/>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-    </row>
-    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+    </row>
+    <row r="2" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="18">
         <v>0</v>
@@ -637,7 +646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18">
         <v>0</v>
       </c>
@@ -706,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -775,7 +784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -844,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -913,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>4</v>
       </c>
@@ -982,7 +991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>5</v>
       </c>
@@ -1051,7 +1060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>6</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>7</v>
       </c>
@@ -1189,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>8</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -1327,7 +1336,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="16" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" s="16" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1352,36 +1361,36 @@
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="15" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
+    <row r="15" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
       <c r="L15" s="13"/>
-      <c r="N15" s="25" t="s">
+      <c r="N15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-    </row>
-    <row r="16" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+    </row>
+    <row r="16" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="18">
         <v>0</v>
@@ -1446,7 +1455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>0</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
         <v>1</v>
       </c>
@@ -1584,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
         <v>2</v>
       </c>
@@ -1653,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>3</v>
       </c>
@@ -1722,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>4</v>
       </c>
@@ -1791,7 +1800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
         <v>5</v>
       </c>
@@ -1860,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>6</v>
       </c>
@@ -1929,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>7</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18">
         <v>8</v>
       </c>
@@ -2067,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>9</v>
       </c>
@@ -2136,36 +2145,36 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
+    <row r="28" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
       <c r="L28" s="13"/>
-      <c r="N28" s="25" t="s">
+      <c r="N28" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="25"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
-      <c r="W28" s="25"/>
-      <c r="X28" s="25"/>
-    </row>
-    <row r="29" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+    </row>
+    <row r="29" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
       <c r="B29" s="18">
         <v>0</v>
@@ -2230,7 +2239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18">
         <v>0</v>
       </c>
@@ -2299,7 +2308,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>1</v>
       </c>
@@ -2368,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18">
         <v>2</v>
       </c>
@@ -2437,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18">
         <v>3</v>
       </c>
@@ -2506,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18">
         <v>4</v>
       </c>
@@ -2575,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18">
         <v>5</v>
       </c>
@@ -2644,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18">
         <v>6</v>
       </c>
@@ -2713,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="18">
         <v>7</v>
       </c>
@@ -2782,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18">
         <v>8</v>
       </c>
@@ -2851,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18">
         <v>9</v>
       </c>
@@ -2920,7 +2929,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -2934,36 +2943,36 @@
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
     </row>
-    <row r="41" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+    <row r="41" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
       <c r="L41" s="13"/>
-      <c r="N41" s="25" t="s">
+      <c r="N41" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-    </row>
-    <row r="42" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+    </row>
+    <row r="42" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="19"/>
       <c r="B42" s="18">
         <v>0</v>
@@ -3028,7 +3037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18">
         <v>0</v>
       </c>
@@ -3097,7 +3106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18">
         <v>1</v>
       </c>
@@ -3166,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18">
         <v>2</v>
       </c>
@@ -3235,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18">
         <v>3</v>
       </c>
@@ -3304,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18">
         <v>4</v>
       </c>
@@ -3373,7 +3382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18">
         <v>5</v>
       </c>
@@ -3442,7 +3451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="18">
         <v>6</v>
       </c>
@@ -3511,7 +3520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18">
         <v>7</v>
       </c>
@@ -3580,7 +3589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18">
         <v>8</v>
       </c>
@@ -3649,7 +3658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18">
         <v>9</v>
       </c>
@@ -3718,35 +3727,35 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+    <row r="54" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="N54" s="25" t="s">
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="N54" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="O54" s="25"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="25"/>
-      <c r="T54" s="25"/>
-      <c r="U54" s="25"/>
-      <c r="V54" s="25"/>
-      <c r="W54" s="25"/>
-      <c r="X54" s="25"/>
-    </row>
-    <row r="55" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
+      <c r="Q54" s="26"/>
+      <c r="R54" s="26"/>
+      <c r="S54" s="26"/>
+      <c r="T54" s="26"/>
+      <c r="U54" s="26"/>
+      <c r="V54" s="26"/>
+      <c r="W54" s="26"/>
+      <c r="X54" s="26"/>
+    </row>
+    <row r="55" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="19"/>
       <c r="B55" s="18">
         <v>0</v>
@@ -3810,7 +3819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18">
         <v>0</v>
       </c>
@@ -3878,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="18">
         <v>1</v>
       </c>
@@ -3946,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18">
         <v>2</v>
       </c>
@@ -4014,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="18">
         <v>3</v>
       </c>
@@ -4082,7 +4091,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18">
         <v>4</v>
       </c>
@@ -4150,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="18">
         <v>5</v>
       </c>
@@ -4218,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18">
         <v>6</v>
       </c>
@@ -4286,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="18">
         <v>7</v>
       </c>
@@ -4354,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18">
         <v>8</v>
       </c>
@@ -4422,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="18">
         <v>9</v>
       </c>
@@ -4490,35 +4499,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="25" t="s">
+    <row r="68" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
-      <c r="I68" s="25"/>
-      <c r="J68" s="25"/>
-      <c r="K68" s="25"/>
-      <c r="N68" s="25" t="s">
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="26"/>
+      <c r="N68" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="O68" s="25"/>
-      <c r="P68" s="25"/>
-      <c r="Q68" s="25"/>
-      <c r="R68" s="25"/>
-      <c r="S68" s="25"/>
-      <c r="T68" s="25"/>
-      <c r="U68" s="25"/>
-      <c r="V68" s="25"/>
-      <c r="W68" s="25"/>
-      <c r="X68" s="25"/>
-    </row>
-    <row r="69" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O68" s="26"/>
+      <c r="P68" s="26"/>
+      <c r="Q68" s="26"/>
+      <c r="R68" s="26"/>
+      <c r="S68" s="26"/>
+      <c r="T68" s="26"/>
+      <c r="U68" s="26"/>
+      <c r="V68" s="26"/>
+      <c r="W68" s="26"/>
+      <c r="X68" s="26"/>
+    </row>
+    <row r="69" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="19"/>
       <c r="B69" s="18">
         <v>0</v>
@@ -4582,7 +4591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="18">
         <v>0</v>
       </c>
@@ -4619,7 +4628,7 @@
       <c r="N70" s="18">
         <v>0</v>
       </c>
-      <c r="O70" s="26">
+      <c r="O70" s="25">
         <v>178</v>
       </c>
       <c r="P70" s="2">
@@ -4650,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18">
         <v>1</v>
       </c>
@@ -4690,7 +4699,7 @@
       <c r="O71" s="2">
         <v>0</v>
       </c>
-      <c r="P71" s="26">
+      <c r="P71" s="25">
         <v>182</v>
       </c>
       <c r="Q71" s="2">
@@ -4718,7 +4727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="18">
         <v>2</v>
       </c>
@@ -4761,7 +4770,7 @@
       <c r="P72" s="2">
         <v>0</v>
       </c>
-      <c r="Q72" s="26">
+      <c r="Q72" s="25">
         <v>176</v>
       </c>
       <c r="R72" s="2">
@@ -4786,7 +4795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="18">
         <v>3</v>
       </c>
@@ -4832,7 +4841,7 @@
       <c r="Q73" s="2">
         <v>0</v>
       </c>
-      <c r="R73" s="26">
+      <c r="R73" s="25">
         <v>178</v>
       </c>
       <c r="S73" s="2">
@@ -4854,7 +4863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="18">
         <v>4</v>
       </c>
@@ -4903,7 +4912,7 @@
       <c r="R74" s="2">
         <v>0</v>
       </c>
-      <c r="S74" s="26">
+      <c r="S74" s="25">
         <v>180</v>
       </c>
       <c r="T74" s="2">
@@ -4922,7 +4931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="18">
         <v>5</v>
       </c>
@@ -4974,7 +4983,7 @@
       <c r="S75" s="2">
         <v>0</v>
       </c>
-      <c r="T75" s="26">
+      <c r="T75" s="25">
         <v>181</v>
       </c>
       <c r="U75" s="2">
@@ -4990,7 +4999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="18">
         <v>6</v>
       </c>
@@ -5045,7 +5054,7 @@
       <c r="T76" s="2">
         <v>0</v>
       </c>
-      <c r="U76" s="26">
+      <c r="U76" s="25">
         <v>180</v>
       </c>
       <c r="V76" s="2">
@@ -5058,7 +5067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="18">
         <v>7</v>
       </c>
@@ -5116,7 +5125,7 @@
       <c r="U77" s="2">
         <v>0</v>
       </c>
-      <c r="V77" s="26">
+      <c r="V77" s="25">
         <v>174</v>
       </c>
       <c r="W77" s="2">
@@ -5126,7 +5135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="18">
         <v>8</v>
       </c>
@@ -5187,14 +5196,14 @@
       <c r="V78" s="2">
         <v>0</v>
       </c>
-      <c r="W78" s="26">
+      <c r="W78" s="25">
         <v>166</v>
       </c>
       <c r="X78" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="18">
         <v>9</v>
       </c>
@@ -5258,24 +5267,24 @@
       <c r="W79" s="2">
         <v>2</v>
       </c>
-      <c r="X79" s="26">
+      <c r="X79" s="25">
         <v>175</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="N54:X54"/>
+    <mergeCell ref="N28:X28"/>
+    <mergeCell ref="N41:X41"/>
+    <mergeCell ref="N68:X68"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="N1:X1"/>
     <mergeCell ref="A41:K41"/>
     <mergeCell ref="N15:X15"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="N54:X54"/>
-    <mergeCell ref="N28:X28"/>
-    <mergeCell ref="N41:X41"/>
-    <mergeCell ref="N68:X68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5284,49 +5293,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y84"/>
+  <dimension ref="A1:AJ84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="Z85" sqref="Z85"/>
+    <sheetView tabSelected="1" topLeftCell="M29" workbookViewId="0">
+      <selection activeCell="AD32" sqref="AD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="11" width="5" style="1"/>
     <col min="12" max="12" width="5" style="16"/>
     <col min="13" max="16384" width="5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+    <row r="1" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="13"/>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-    </row>
-    <row r="2" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+    </row>
+    <row r="2" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="18">
         <v>0</v>
@@ -5391,7 +5400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18">
         <v>0</v>
       </c>
@@ -5467,7 +5476,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -5543,7 +5552,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -5619,7 +5628,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -5695,7 +5704,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>4</v>
       </c>
@@ -5771,7 +5780,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>5</v>
       </c>
@@ -5847,7 +5856,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>6</v>
       </c>
@@ -5923,7 +5932,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>7</v>
       </c>
@@ -5999,7 +6008,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>8</v>
       </c>
@@ -6075,7 +6084,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -6151,7 +6160,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="16" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" s="16" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23"/>
       <c r="B13" s="13">
         <f t="shared" ref="B13:K13" si="2">SUM(B3:B12)</f>
@@ -6243,7 +6252,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L14" s="1">
         <v>1648</v>
       </c>
@@ -6251,36 +6260,36 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
+    <row r="15" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
       <c r="L15" s="13"/>
-      <c r="N15" s="25" t="s">
+      <c r="N15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-    </row>
-    <row r="16" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+    </row>
+    <row r="16" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="18">
         <v>0</v>
@@ -6345,7 +6354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>0</v>
       </c>
@@ -6421,7 +6430,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
         <v>1</v>
       </c>
@@ -6497,7 +6506,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
         <v>2</v>
       </c>
@@ -6573,7 +6582,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>3</v>
       </c>
@@ -6649,7 +6658,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>4</v>
       </c>
@@ -6725,7 +6734,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
         <v>5</v>
       </c>
@@ -6801,7 +6810,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>6</v>
       </c>
@@ -6877,7 +6886,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>7</v>
       </c>
@@ -6953,7 +6962,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18">
         <v>8</v>
       </c>
@@ -7029,7 +7038,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>9</v>
       </c>
@@ -7105,7 +7114,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20"/>
       <c r="B27" s="24">
         <f t="shared" ref="B27:K27" si="6">SUM(B17:B26)</f>
@@ -7197,7 +7206,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L28" s="16">
         <v>1744</v>
       </c>
@@ -7205,36 +7214,36 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
+    <row r="29" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
       <c r="L29" s="13"/>
-      <c r="N29" s="25" t="s">
+      <c r="N29" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="25"/>
-    </row>
-    <row r="30" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+    </row>
+    <row r="30" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17"/>
       <c r="B30" s="18">
         <v>0</v>
@@ -7298,8 +7307,20 @@
       <c r="X30" s="18">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA30" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27"/>
+      <c r="AD30" s="27"/>
+      <c r="AE30" s="27"/>
+      <c r="AF30" s="27"/>
+      <c r="AG30" s="27"/>
+      <c r="AH30" s="27"/>
+      <c r="AI30" s="27"/>
+      <c r="AJ30" s="27"/>
+    </row>
+    <row r="31" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>0</v>
       </c>
@@ -7374,8 +7395,19 @@
         <f t="shared" ref="Y31:Y41" si="9">SUM(O31:X31)</f>
         <v>901</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA31" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB31" s="27"/>
+      <c r="AC31" s="27"/>
+      <c r="AD31" s="27"/>
+      <c r="AE31" s="27"/>
+      <c r="AF31" s="27"/>
+      <c r="AG31" s="27"/>
+      <c r="AH31" s="27"/>
+      <c r="AI31" s="27"/>
+    </row>
+    <row r="32" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18">
         <v>1</v>
       </c>
@@ -7451,7 +7483,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18">
         <v>2</v>
       </c>
@@ -7527,7 +7559,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18">
         <v>3</v>
       </c>
@@ -7603,7 +7635,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18">
         <v>4</v>
       </c>
@@ -7679,7 +7711,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18">
         <v>5</v>
       </c>
@@ -7755,7 +7787,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="18">
         <v>6</v>
       </c>
@@ -7831,7 +7863,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18">
         <v>7</v>
       </c>
@@ -7907,7 +7939,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18">
         <v>8</v>
       </c>
@@ -7983,7 +8015,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18">
         <v>9</v>
       </c>
@@ -8059,7 +8091,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="20"/>
       <c r="B41" s="11">
         <f t="shared" ref="B41:K41" si="10">SUM(B31:B40)</f>
@@ -8151,7 +8183,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -8170,36 +8202,36 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+    <row r="43" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
       <c r="L43" s="13"/>
-      <c r="N43" s="25" t="s">
+      <c r="N43" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="O43" s="25"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="25"/>
-      <c r="T43" s="25"/>
-      <c r="U43" s="25"/>
-      <c r="V43" s="25"/>
-      <c r="W43" s="25"/>
-      <c r="X43" s="25"/>
-    </row>
-    <row r="44" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="26"/>
+      <c r="T43" s="26"/>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+    </row>
+    <row r="44" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="19"/>
       <c r="B44" s="18">
         <v>0</v>
@@ -8264,7 +8296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18">
         <v>0</v>
       </c>
@@ -8340,7 +8372,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18">
         <v>1</v>
       </c>
@@ -8416,7 +8448,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18">
         <v>2</v>
       </c>
@@ -8492,7 +8524,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18">
         <v>3</v>
       </c>
@@ -8568,7 +8600,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="18">
         <v>4</v>
       </c>
@@ -8644,7 +8676,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18">
         <v>5</v>
       </c>
@@ -8720,7 +8752,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18">
         <v>6</v>
       </c>
@@ -8796,7 +8828,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18">
         <v>7</v>
       </c>
@@ -8872,7 +8904,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18">
         <v>8</v>
       </c>
@@ -8948,7 +8980,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18">
         <v>9</v>
       </c>
@@ -9024,7 +9056,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="1">
         <f t="shared" ref="B55:K55" si="14">SUM(B45:B54)</f>
         <v>178</v>
@@ -9114,7 +9146,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L56" s="16">
         <v>1735</v>
       </c>
@@ -9122,36 +9154,36 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
+    <row r="58" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="25"/>
-      <c r="N58" s="25" t="s">
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="N58" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="O58" s="25"/>
-      <c r="P58" s="25"/>
-      <c r="Q58" s="25"/>
-      <c r="R58" s="25"/>
-      <c r="S58" s="25"/>
-      <c r="T58" s="25"/>
-      <c r="U58" s="25"/>
-      <c r="V58" s="25"/>
-      <c r="W58" s="25"/>
-      <c r="X58" s="25"/>
+      <c r="O58" s="26"/>
+      <c r="P58" s="26"/>
+      <c r="Q58" s="26"/>
+      <c r="R58" s="26"/>
+      <c r="S58" s="26"/>
+      <c r="T58" s="26"/>
+      <c r="U58" s="26"/>
+      <c r="V58" s="26"/>
+      <c r="W58" s="26"/>
+      <c r="X58" s="26"/>
       <c r="Y58" s="16"/>
     </row>
-    <row r="59" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="19"/>
       <c r="B59" s="18">
         <v>0</v>
@@ -9216,7 +9248,7 @@
       </c>
       <c r="Y59" s="16"/>
     </row>
-    <row r="60" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18">
         <v>0</v>
       </c>
@@ -9292,7 +9324,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="18">
         <v>1</v>
       </c>
@@ -9368,7 +9400,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18">
         <v>2</v>
       </c>
@@ -9444,7 +9476,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="18">
         <v>3</v>
       </c>
@@ -9520,7 +9552,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18">
         <v>4</v>
       </c>
@@ -9596,7 +9628,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="18">
         <v>5</v>
       </c>
@@ -9672,7 +9704,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="18">
         <v>6</v>
       </c>
@@ -9748,7 +9780,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="18">
         <v>7</v>
       </c>
@@ -9824,7 +9856,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="18">
         <v>8</v>
       </c>
@@ -9900,7 +9932,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="18">
         <v>9</v>
       </c>
@@ -9976,7 +10008,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="1">
         <f t="shared" ref="B70:K70" si="18">SUM(B60:B69)</f>
         <v>178</v>
@@ -10066,35 +10098,35 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="25" t="s">
+    <row r="72" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
-      <c r="H72" s="25"/>
-      <c r="I72" s="25"/>
-      <c r="J72" s="25"/>
-      <c r="K72" s="25"/>
-      <c r="N72" s="25" t="s">
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="26"/>
+      <c r="I72" s="26"/>
+      <c r="J72" s="26"/>
+      <c r="K72" s="26"/>
+      <c r="N72" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="O72" s="25"/>
-      <c r="P72" s="25"/>
-      <c r="Q72" s="25"/>
-      <c r="R72" s="25"/>
-      <c r="S72" s="25"/>
-      <c r="T72" s="25"/>
-      <c r="U72" s="25"/>
-      <c r="V72" s="25"/>
-      <c r="W72" s="25"/>
-      <c r="X72" s="25"/>
-    </row>
-    <row r="73" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O72" s="26"/>
+      <c r="P72" s="26"/>
+      <c r="Q72" s="26"/>
+      <c r="R72" s="26"/>
+      <c r="S72" s="26"/>
+      <c r="T72" s="26"/>
+      <c r="U72" s="26"/>
+      <c r="V72" s="26"/>
+      <c r="W72" s="26"/>
+      <c r="X72" s="26"/>
+    </row>
+    <row r="73" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="19"/>
       <c r="B73" s="18">
         <v>0</v>
@@ -10158,7 +10190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="18">
         <v>0</v>
       </c>
@@ -10195,7 +10227,7 @@
       <c r="N74" s="18">
         <v>0</v>
       </c>
-      <c r="O74" s="26">
+      <c r="O74" s="25">
         <v>178</v>
       </c>
       <c r="P74" s="2">
@@ -10226,11 +10258,11 @@
         <v>0</v>
       </c>
       <c r="Y74" s="1">
-        <f>SUM(O74:X74)</f>
+        <f t="shared" ref="Y74:Y84" si="20">SUM(O74:X74)</f>
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="18">
         <v>1</v>
       </c>
@@ -10270,7 +10302,7 @@
       <c r="O75" s="2">
         <v>0</v>
       </c>
-      <c r="P75" s="26">
+      <c r="P75" s="25">
         <v>182</v>
       </c>
       <c r="Q75" s="2">
@@ -10298,11 +10330,11 @@
         <v>1</v>
       </c>
       <c r="Y75" s="1">
-        <f>SUM(O75:X75)</f>
+        <f t="shared" si="20"/>
         <v>190</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="18">
         <v>2</v>
       </c>
@@ -10345,7 +10377,7 @@
       <c r="P76" s="2">
         <v>0</v>
       </c>
-      <c r="Q76" s="26">
+      <c r="Q76" s="25">
         <v>176</v>
       </c>
       <c r="R76" s="2">
@@ -10370,11 +10402,11 @@
         <v>0</v>
       </c>
       <c r="Y76" s="1">
-        <f>SUM(O76:X76)</f>
+        <f t="shared" si="20"/>
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="18">
         <v>3</v>
       </c>
@@ -10420,7 +10452,7 @@
       <c r="Q77" s="2">
         <v>0</v>
       </c>
-      <c r="R77" s="26">
+      <c r="R77" s="25">
         <v>178</v>
       </c>
       <c r="S77" s="2">
@@ -10442,11 +10474,11 @@
         <v>1</v>
       </c>
       <c r="Y77" s="1">
-        <f>SUM(O77:X77)</f>
+        <f t="shared" si="20"/>
         <v>179</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="18">
         <v>4</v>
       </c>
@@ -10495,7 +10527,7 @@
       <c r="R78" s="2">
         <v>0</v>
       </c>
-      <c r="S78" s="26">
+      <c r="S78" s="25">
         <v>180</v>
       </c>
       <c r="T78" s="2">
@@ -10514,11 +10546,11 @@
         <v>0</v>
       </c>
       <c r="Y78" s="1">
-        <f>SUM(O78:X78)</f>
+        <f t="shared" si="20"/>
         <v>180</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="18">
         <v>5</v>
       </c>
@@ -10570,7 +10602,7 @@
       <c r="S79" s="2">
         <v>0</v>
       </c>
-      <c r="T79" s="26">
+      <c r="T79" s="25">
         <v>181</v>
       </c>
       <c r="U79" s="2">
@@ -10586,11 +10618,11 @@
         <v>1</v>
       </c>
       <c r="Y79" s="1">
-        <f>SUM(O79:X79)</f>
+        <f t="shared" si="20"/>
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="18">
         <v>6</v>
       </c>
@@ -10645,7 +10677,7 @@
       <c r="T80" s="2">
         <v>0</v>
       </c>
-      <c r="U80" s="26">
+      <c r="U80" s="25">
         <v>180</v>
       </c>
       <c r="V80" s="2">
@@ -10658,11 +10690,11 @@
         <v>0</v>
       </c>
       <c r="Y80" s="1">
-        <f>SUM(O80:X80)</f>
+        <f t="shared" si="20"/>
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="18">
         <v>7</v>
       </c>
@@ -10720,7 +10752,7 @@
       <c r="U81" s="2">
         <v>0</v>
       </c>
-      <c r="V81" s="26">
+      <c r="V81" s="25">
         <v>174</v>
       </c>
       <c r="W81" s="2">
@@ -10730,11 +10762,11 @@
         <v>0</v>
       </c>
       <c r="Y81" s="1">
-        <f>SUM(O81:X81)</f>
+        <f t="shared" si="20"/>
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="18">
         <v>8</v>
       </c>
@@ -10795,18 +10827,18 @@
       <c r="V82" s="2">
         <v>0</v>
       </c>
-      <c r="W82" s="26">
+      <c r="W82" s="25">
         <v>166</v>
       </c>
       <c r="X82" s="2">
         <v>2</v>
       </c>
       <c r="Y82" s="1">
-        <f>SUM(O82:X82)</f>
+        <f t="shared" si="20"/>
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="18">
         <v>9</v>
       </c>
@@ -10870,74 +10902,76 @@
       <c r="W83" s="2">
         <v>2</v>
       </c>
-      <c r="X83" s="26">
+      <c r="X83" s="25">
         <v>175</v>
       </c>
       <c r="Y83" s="1">
-        <f>SUM(O83:X83)</f>
+        <f t="shared" si="20"/>
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O84" s="1">
-        <f>SUM(O74:O83)</f>
+        <f t="shared" ref="O84:X84" si="21">SUM(O74:O83)</f>
         <v>178</v>
       </c>
       <c r="P84" s="1">
-        <f>SUM(P74:P83)</f>
+        <f t="shared" si="21"/>
         <v>182</v>
       </c>
       <c r="Q84" s="1">
-        <f>SUM(Q74:Q83)</f>
+        <f t="shared" si="21"/>
         <v>177</v>
       </c>
       <c r="R84" s="1">
-        <f>SUM(R74:R83)</f>
+        <f t="shared" si="21"/>
         <v>183</v>
       </c>
       <c r="S84" s="1">
-        <f>SUM(S74:S83)</f>
+        <f t="shared" si="21"/>
         <v>181</v>
       </c>
       <c r="T84" s="1">
-        <f>SUM(T74:T83)</f>
+        <f t="shared" si="21"/>
         <v>182</v>
       </c>
       <c r="U84" s="1">
-        <f>SUM(U74:U83)</f>
+        <f t="shared" si="21"/>
         <v>181</v>
       </c>
       <c r="V84" s="1">
-        <f>SUM(V74:V83)</f>
+        <f t="shared" si="21"/>
         <v>179</v>
       </c>
       <c r="W84" s="1">
-        <f>SUM(W74:W83)</f>
+        <f t="shared" si="21"/>
         <v>174</v>
       </c>
       <c r="X84" s="1">
-        <f>SUM(X74:X83)</f>
+        <f t="shared" si="21"/>
         <v>180</v>
       </c>
       <c r="Y84" s="1">
-        <f>SUM(O84:X84)</f>
+        <f t="shared" si="20"/>
         <v>1797</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="AA30:AJ30"/>
+    <mergeCell ref="AA31:AI31"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="N58:X58"/>
+    <mergeCell ref="A72:K72"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="N43:X43"/>
+    <mergeCell ref="N72:X72"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="N1:X1"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="N15:X15"/>
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="N29:X29"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="N58:X58"/>
-    <mergeCell ref="A72:K72"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="N43:X43"/>
-    <mergeCell ref="N72:X72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>